<commit_message>
41???? HS circuits data
</commit_message>
<xml_diff>
--- a/ExecutionData.xlsx
+++ b/ExecutionData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/psantos/QCircuits_BenchTest/circuits/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4052A476-0DE6-6D4E-84FA-17D7AE3FF176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F109B7-256F-6F4F-9A97-F72B1E317D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{E6CD9D0F-01ED-C84F-820F-C3D6AE701B6F}"/>
   </bookViews>
@@ -488,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35810972-CC3A-EC4D-BC0F-849D914B767C}">
-  <dimension ref="B3:AD18"/>
+  <dimension ref="B3:AD34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AD19" sqref="AD19"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="V29" sqref="V29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1701,6 +1701,1017 @@
         <v>4.0178659999999996E-6</v>
       </c>
     </row>
+    <row r="20" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>4110</v>
+      </c>
+      <c r="C20">
+        <v>10</v>
+      </c>
+      <c r="D20">
+        <v>56</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>12</v>
+      </c>
+      <c r="H20">
+        <v>25</v>
+      </c>
+      <c r="I20">
+        <v>14718566</v>
+      </c>
+      <c r="J20">
+        <v>33554432</v>
+      </c>
+      <c r="K20">
+        <v>131300</v>
+      </c>
+      <c r="L20">
+        <v>1.007598</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20" s="2">
+        <v>5.77296039999999E-5</v>
+      </c>
+      <c r="O20">
+        <v>12</v>
+      </c>
+      <c r="P20">
+        <v>23</v>
+      </c>
+      <c r="Q20">
+        <v>11636162</v>
+      </c>
+      <c r="R20">
+        <v>469762048</v>
+      </c>
+      <c r="S20">
+        <v>818420</v>
+      </c>
+      <c r="T20">
+        <v>0.998108</v>
+      </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
+      <c r="V20" s="2">
+        <v>3.5796640000000098E-6</v>
+      </c>
+      <c r="W20">
+        <v>12</v>
+      </c>
+      <c r="X20">
+        <v>20</v>
+      </c>
+      <c r="Y20">
+        <v>1027858</v>
+      </c>
+      <c r="Z20">
+        <v>58720256</v>
+      </c>
+      <c r="AA20">
+        <v>102760</v>
+      </c>
+      <c r="AB20">
+        <v>0.99820299999999995</v>
+      </c>
+      <c r="AC20">
+        <v>0</v>
+      </c>
+      <c r="AD20" s="2">
+        <v>3.2292090000001698E-6</v>
+      </c>
+    </row>
+    <row r="21" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <v>4120</v>
+      </c>
+      <c r="C21">
+        <v>20</v>
+      </c>
+      <c r="D21">
+        <v>46</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>12</v>
+      </c>
+      <c r="H21">
+        <v>25</v>
+      </c>
+      <c r="I21">
+        <v>24611442</v>
+      </c>
+      <c r="J21">
+        <v>33554432</v>
+      </c>
+      <c r="K21">
+        <v>70</v>
+      </c>
+      <c r="L21">
+        <v>1.3124990000000001</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21" s="2">
+        <v>9.7655625001000002E-2</v>
+      </c>
+      <c r="O21">
+        <v>12</v>
+      </c>
+      <c r="P21">
+        <v>23</v>
+      </c>
+      <c r="Q21">
+        <v>18969214</v>
+      </c>
+      <c r="R21">
+        <v>377487360</v>
+      </c>
+      <c r="S21">
+        <v>21997</v>
+      </c>
+      <c r="T21">
+        <v>0.74482899999999996</v>
+      </c>
+      <c r="U21">
+        <v>0</v>
+      </c>
+      <c r="V21">
+        <v>6.5112239241E-2</v>
+      </c>
+      <c r="W21">
+        <v>12</v>
+      </c>
+      <c r="X21">
+        <v>22</v>
+      </c>
+      <c r="Y21">
+        <v>6598495</v>
+      </c>
+      <c r="Z21">
+        <v>188743680</v>
+      </c>
+      <c r="AA21">
+        <v>10832</v>
+      </c>
+      <c r="AB21">
+        <v>0.98109000000000002</v>
+      </c>
+      <c r="AC21">
+        <v>0</v>
+      </c>
+      <c r="AD21" s="2">
+        <v>3.57588099999999E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <v>4130</v>
+      </c>
+      <c r="C22">
+        <v>30</v>
+      </c>
+      <c r="D22">
+        <v>43</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>24</v>
+      </c>
+      <c r="H22">
+        <v>26</v>
+      </c>
+      <c r="I22">
+        <v>30388334</v>
+      </c>
+      <c r="J22">
+        <v>67108864</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <v>7.9999900000000004</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22" s="2">
+        <v>48.9998600001</v>
+      </c>
+      <c r="O22">
+        <v>24</v>
+      </c>
+      <c r="P22">
+        <v>24</v>
+      </c>
+      <c r="Q22">
+        <v>18782562</v>
+      </c>
+      <c r="R22">
+        <v>721420288</v>
+      </c>
+      <c r="S22">
+        <v>4241</v>
+      </c>
+      <c r="T22">
+        <v>7.0290000000000005E-2</v>
+      </c>
+      <c r="U22">
+        <v>0</v>
+      </c>
+      <c r="V22">
+        <v>0.8643606841</v>
+      </c>
+      <c r="W22">
+        <v>12</v>
+      </c>
+      <c r="X22">
+        <v>22</v>
+      </c>
+      <c r="Y22">
+        <v>12956592</v>
+      </c>
+      <c r="Z22">
+        <v>180355072</v>
+      </c>
+      <c r="AA22">
+        <v>1074</v>
+      </c>
+      <c r="AB22">
+        <v>1.0128779999999999</v>
+      </c>
+      <c r="AC22">
+        <v>0</v>
+      </c>
+      <c r="AD22" s="2">
+        <v>1.6584288399999799E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <v>4140</v>
+      </c>
+      <c r="C23">
+        <v>40</v>
+      </c>
+      <c r="D23">
+        <v>43</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>24</v>
+      </c>
+      <c r="H23">
+        <v>26</v>
+      </c>
+      <c r="I23">
+        <v>36919968</v>
+      </c>
+      <c r="J23">
+        <v>67108864</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23" s="2">
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <v>24</v>
+      </c>
+      <c r="P23">
+        <v>24</v>
+      </c>
+      <c r="Q23">
+        <v>24646975</v>
+      </c>
+      <c r="R23">
+        <v>721420288</v>
+      </c>
+      <c r="S23">
+        <v>2066</v>
+      </c>
+      <c r="T23">
+        <v>4.7238000000000002E-2</v>
+      </c>
+      <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="V23">
+        <v>0.90775542864400005</v>
+      </c>
+      <c r="W23">
+        <v>24</v>
+      </c>
+      <c r="X23">
+        <v>23</v>
+      </c>
+      <c r="Y23">
+        <v>11990607</v>
+      </c>
+      <c r="Z23">
+        <v>360710144</v>
+      </c>
+      <c r="AA23">
+        <v>1032</v>
+      </c>
+      <c r="AB23">
+        <v>1.0175339999999999</v>
+      </c>
+      <c r="AC23">
+        <v>0</v>
+      </c>
+      <c r="AD23" s="2">
+        <v>3.0744115599999698E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B24">
+        <v>4150</v>
+      </c>
+      <c r="C24">
+        <v>50</v>
+      </c>
+      <c r="D24">
+        <v>43</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>48</v>
+      </c>
+      <c r="H24">
+        <v>26</v>
+      </c>
+      <c r="I24">
+        <v>21026295</v>
+      </c>
+      <c r="J24">
+        <v>67108864</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24" s="2">
+        <v>1</v>
+      </c>
+      <c r="O24">
+        <v>48</v>
+      </c>
+      <c r="P24">
+        <v>24</v>
+      </c>
+      <c r="Q24">
+        <v>14077201</v>
+      </c>
+      <c r="R24">
+        <v>721420288</v>
+      </c>
+      <c r="S24">
+        <v>1001</v>
+      </c>
+      <c r="T24">
+        <v>2.3892E-2</v>
+      </c>
+      <c r="U24">
+        <v>0</v>
+      </c>
+      <c r="V24">
+        <v>0.95278682766399903</v>
+      </c>
+      <c r="W24">
+        <v>48</v>
+      </c>
+      <c r="X24">
+        <v>24</v>
+      </c>
+      <c r="Y24">
+        <v>9954197</v>
+      </c>
+      <c r="Z24">
+        <v>721420288</v>
+      </c>
+      <c r="AA24">
+        <v>1035</v>
+      </c>
+      <c r="AB24">
+        <v>1.0643210000000001</v>
+      </c>
+      <c r="AC24">
+        <v>0</v>
+      </c>
+      <c r="AD24" s="2">
+        <v>4.1371910410000004E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B25">
+        <v>4160</v>
+      </c>
+      <c r="C25">
+        <v>60</v>
+      </c>
+      <c r="D25">
+        <v>43</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>48</v>
+      </c>
+      <c r="H25">
+        <v>27</v>
+      </c>
+      <c r="I25">
+        <v>49055885</v>
+      </c>
+      <c r="J25">
+        <v>134217728</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25" s="2">
+        <v>1</v>
+      </c>
+      <c r="O25">
+        <v>48</v>
+      </c>
+      <c r="P25">
+        <v>25</v>
+      </c>
+      <c r="Q25">
+        <v>33069298</v>
+      </c>
+      <c r="R25">
+        <v>1442840576</v>
+      </c>
+      <c r="S25">
+        <v>2023</v>
+      </c>
+      <c r="T25">
+        <v>2.3050999999999999E-2</v>
+      </c>
+      <c r="U25">
+        <v>0</v>
+      </c>
+      <c r="V25">
+        <v>0.95442934860099904</v>
+      </c>
+      <c r="W25">
+        <v>48</v>
+      </c>
+      <c r="X25">
+        <v>25</v>
+      </c>
+      <c r="Y25">
+        <v>27087351</v>
+      </c>
+      <c r="Z25">
+        <v>1442840576</v>
+      </c>
+      <c r="AA25">
+        <v>2065</v>
+      </c>
+      <c r="AB25">
+        <v>1.06054</v>
+      </c>
+      <c r="AC25">
+        <v>0</v>
+      </c>
+      <c r="AD25" s="2">
+        <v>3.6650915999999999E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B26">
+        <v>4170</v>
+      </c>
+      <c r="C26">
+        <v>70</v>
+      </c>
+      <c r="D26">
+        <v>43</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>48</v>
+      </c>
+      <c r="H26">
+        <v>27</v>
+      </c>
+      <c r="I26">
+        <v>2510414007</v>
+      </c>
+      <c r="J26">
+        <v>134217728</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26" s="2">
+        <v>1</v>
+      </c>
+      <c r="O26">
+        <v>48</v>
+      </c>
+      <c r="P26">
+        <v>27</v>
+      </c>
+      <c r="Q26">
+        <v>6725957087</v>
+      </c>
+      <c r="R26">
+        <v>5771362304</v>
+      </c>
+      <c r="S26">
+        <v>4159</v>
+      </c>
+      <c r="T26">
+        <v>2.3494000000000001E-2</v>
+      </c>
+      <c r="U26">
+        <v>0</v>
+      </c>
+      <c r="V26">
+        <v>0.95356396803599996</v>
+      </c>
+      <c r="W26">
+        <v>48</v>
+      </c>
+      <c r="X26">
+        <v>27</v>
+      </c>
+      <c r="Y26">
+        <v>7298131536</v>
+      </c>
+      <c r="Z26">
+        <v>5771362304</v>
+      </c>
+      <c r="AA26">
+        <v>4237</v>
+      </c>
+      <c r="AB26">
+        <v>1.006589</v>
+      </c>
+      <c r="AC26">
+        <v>0</v>
+      </c>
+      <c r="AD26" s="2">
+        <v>4.3414920999999398E-5</v>
+      </c>
+    </row>
+    <row r="27" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B27">
+        <v>4180</v>
+      </c>
+      <c r="C27">
+        <v>80</v>
+      </c>
+      <c r="D27">
+        <v>43</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>48</v>
+      </c>
+      <c r="H27">
+        <v>28</v>
+      </c>
+      <c r="I27">
+        <v>4310433172</v>
+      </c>
+      <c r="J27">
+        <v>268435456</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27" s="2">
+        <v>1</v>
+      </c>
+      <c r="O27">
+        <v>48</v>
+      </c>
+      <c r="P27">
+        <v>28</v>
+      </c>
+      <c r="Q27">
+        <v>235737241</v>
+      </c>
+      <c r="R27">
+        <v>11542724608</v>
+      </c>
+      <c r="S27">
+        <v>8117</v>
+      </c>
+      <c r="T27">
+        <v>2.3241999999999999E-2</v>
+      </c>
+      <c r="U27">
+        <v>0</v>
+      </c>
+      <c r="V27">
+        <v>0.95405619056400004</v>
+      </c>
+      <c r="W27">
+        <v>48</v>
+      </c>
+      <c r="X27">
+        <v>28</v>
+      </c>
+      <c r="Y27">
+        <v>14947210225</v>
+      </c>
+      <c r="Z27">
+        <v>11542724608</v>
+      </c>
+      <c r="AA27">
+        <v>8241</v>
+      </c>
+      <c r="AB27">
+        <v>1.003171</v>
+      </c>
+      <c r="AC27">
+        <v>0</v>
+      </c>
+      <c r="AD27" s="2">
+        <v>1.00552410000002E-5</v>
+      </c>
+    </row>
+    <row r="28" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B28">
+        <v>4190</v>
+      </c>
+      <c r="C28">
+        <v>90</v>
+      </c>
+      <c r="D28">
+        <v>43</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <v>8</v>
+      </c>
+      <c r="P28">
+        <v>24</v>
+      </c>
+      <c r="Q28">
+        <v>56471654</v>
+      </c>
+      <c r="R28">
+        <v>721420288</v>
+      </c>
+      <c r="T28">
+        <v>2.2075000000000001E-2</v>
+      </c>
+      <c r="U28">
+        <v>0</v>
+      </c>
+      <c r="V28">
+        <v>0.95633800000000002</v>
+      </c>
+      <c r="W28">
+        <v>8</v>
+      </c>
+      <c r="X28">
+        <v>24</v>
+      </c>
+      <c r="Y28">
+        <v>2720944519</v>
+      </c>
+      <c r="Z28">
+        <v>721420288</v>
+      </c>
+      <c r="AB28">
+        <v>0.94530899999999995</v>
+      </c>
+      <c r="AC28">
+        <v>0</v>
+      </c>
+      <c r="AD28" s="2">
+        <v>2.9910000000000002E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B29">
+        <v>41120</v>
+      </c>
+      <c r="C29">
+        <v>120</v>
+      </c>
+      <c r="D29">
+        <v>43</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="W29">
+        <v>48</v>
+      </c>
+      <c r="X29">
+        <v>27</v>
+      </c>
+      <c r="Y29">
+        <v>8553062845</v>
+      </c>
+      <c r="Z29">
+        <v>5771362304</v>
+      </c>
+      <c r="AA29">
+        <v>2014</v>
+      </c>
+      <c r="AB29">
+        <v>0.98339399999999999</v>
+      </c>
+      <c r="AC29">
+        <v>0</v>
+      </c>
+      <c r="AD29">
+        <v>2.7599999999999999E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B30">
+        <v>41256</v>
+      </c>
+      <c r="C30">
+        <v>256</v>
+      </c>
+      <c r="D30">
+        <v>43</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="W30">
+        <v>48</v>
+      </c>
+      <c r="X30">
+        <v>28</v>
+      </c>
+      <c r="Y30">
+        <v>33795072369</v>
+      </c>
+      <c r="Z30">
+        <v>11542724608</v>
+      </c>
+      <c r="AA30">
+        <v>8192</v>
+      </c>
+      <c r="AB30">
+        <v>0.99999099999999996</v>
+      </c>
+      <c r="AC30">
+        <v>0</v>
+      </c>
+      <c r="AD30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B31">
+        <v>41512</v>
+      </c>
+      <c r="C31">
+        <v>512</v>
+      </c>
+      <c r="D31">
+        <v>43</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="W31">
+        <v>48</v>
+      </c>
+      <c r="X31">
+        <v>25</v>
+      </c>
+      <c r="Y31">
+        <v>11693644502</v>
+      </c>
+      <c r="Z31">
+        <v>1442840576</v>
+      </c>
+      <c r="AA31">
+        <v>1009</v>
+      </c>
+      <c r="AB31">
+        <v>0.98533400000000004</v>
+      </c>
+      <c r="AC31">
+        <v>0</v>
+      </c>
+      <c r="AD31">
+        <v>2.1499999999999999E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B32">
+        <v>411024</v>
+      </c>
+      <c r="C32">
+        <v>1024</v>
+      </c>
+      <c r="D32">
+        <v>43</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="W32">
+        <v>48</v>
+      </c>
+      <c r="X32">
+        <v>24</v>
+      </c>
+      <c r="Y32">
+        <v>20510047491</v>
+      </c>
+      <c r="Z32">
+        <v>721420288</v>
+      </c>
+      <c r="AB32">
+        <v>1.0331669999999999</v>
+      </c>
+      <c r="AC32">
+        <v>0</v>
+      </c>
+      <c r="AD32">
+        <v>1.1000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B33">
+        <v>412048</v>
+      </c>
+      <c r="C33">
+        <v>2048</v>
+      </c>
+      <c r="D33">
+        <v>43</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="W33">
+        <v>48</v>
+      </c>
+      <c r="X33">
+        <v>24</v>
+      </c>
+      <c r="Y33">
+        <v>41138387598</v>
+      </c>
+      <c r="Z33">
+        <v>721420288</v>
+      </c>
+      <c r="AB33">
+        <v>0.91399799999999998</v>
+      </c>
+      <c r="AC33">
+        <v>0</v>
+      </c>
+      <c r="AD33">
+        <v>7.3959999999999998E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B34">
+        <v>414096</v>
+      </c>
+      <c r="C34">
+        <v>4096</v>
+      </c>
+      <c r="D34">
+        <v>43</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="W34">
+        <v>48</v>
+      </c>
+      <c r="X34">
+        <v>25</v>
+      </c>
+      <c r="Y34">
+        <v>195678067961</v>
+      </c>
+      <c r="Z34">
+        <v>1442840576</v>
+      </c>
+      <c r="AA34">
+        <v>1040</v>
+      </c>
+      <c r="AB34">
+        <v>1.015482</v>
+      </c>
+      <c r="AC34">
+        <v>0</v>
+      </c>
+      <c r="AD34">
+        <v>2.4000000000000001E-4</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="H3:N3"/>

</xml_diff>